<commit_message>
Image resizing, time tracker fixes
</commit_message>
<xml_diff>
--- a/15.3/15.3-timesheet.xlsx
+++ b/15.3/15.3-timesheet.xlsx
@@ -187,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -281,7 +281,6 @@
       <alignment/>
     </xf>
     <xf borderId="0" fillId="5" fontId="6" numFmtId="20" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="20" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="18" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
@@ -656,7 +655,7 @@
         <v>17</v>
       </c>
       <c r="D10" s="25">
-        <v>0.006944444444444444</v>
+        <v>0.010416666666666666</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -684,7 +683,7 @@
     <row r="11">
       <c r="A11" s="26">
         <f t="shared" si="1"/>
-        <v>0.4763888889</v>
+        <v>0.4798611111</v>
       </c>
       <c r="B11" s="27">
         <v>8.0</v>
@@ -723,7 +722,7 @@
     <row r="12">
       <c r="A12" s="24">
         <f t="shared" si="1"/>
-        <v>0.4868055556</v>
+        <v>0.4902777778</v>
       </c>
       <c r="B12" s="19">
         <v>9.0</v>
@@ -760,7 +759,7 @@
     <row r="13">
       <c r="A13" s="24">
         <f t="shared" si="1"/>
-        <v>0.4902777778</v>
+        <v>0.49375</v>
       </c>
       <c r="B13" s="19">
         <v>10.0</v>
@@ -797,7 +796,7 @@
     <row r="14">
       <c r="A14" s="24">
         <f t="shared" si="1"/>
-        <v>0.49375</v>
+        <v>0.4972222222</v>
       </c>
       <c r="B14" s="19"/>
       <c r="C14" s="15" t="s">
@@ -832,7 +831,7 @@
     <row r="15">
       <c r="A15" s="31">
         <f t="shared" si="1"/>
-        <v>0.5215277778</v>
+        <v>0.525</v>
       </c>
       <c r="B15" s="32">
         <v>11.0</v>
@@ -868,7 +867,7 @@
     <row r="16">
       <c r="A16" s="35">
         <f t="shared" si="1"/>
-        <v>0.525</v>
+        <v>0.5284722222</v>
       </c>
       <c r="B16" s="21">
         <v>12.0</v>
@@ -877,7 +876,7 @@
         <v>23</v>
       </c>
       <c r="D16" s="37">
-        <v>0.020833333333333332</v>
+        <v>0.017361111111111112</v>
       </c>
       <c r="E16" s="22" t="s">
         <v>16</v>
@@ -916,7 +915,7 @@
         <v>24</v>
       </c>
       <c r="D17" s="25">
-        <v>0.010416666666666666</v>
+        <v>0.013888888888888888</v>
       </c>
       <c r="E17" s="30"/>
       <c r="F17" s="3"/>
@@ -944,7 +943,7 @@
     <row r="18">
       <c r="A18" s="35">
         <f t="shared" si="1"/>
-        <v>0.55625</v>
+        <v>0.5597222222</v>
       </c>
       <c r="B18" s="21">
         <v>14.0</v>
@@ -953,7 +952,7 @@
         <v>25</v>
       </c>
       <c r="D18" s="37">
-        <v>0.017361111111111112</v>
+        <v>0.013888888888888888</v>
       </c>
       <c r="E18" s="22" t="s">
         <v>16</v>
@@ -1027,7 +1026,7 @@
         <v>27</v>
       </c>
       <c r="D20" s="42"/>
-      <c r="E20" s="43"/>
+      <c r="E20" s="42"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -1082,7 +1081,7 @@
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="44"/>
+      <c r="D22" s="43"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -1110,7 +1109,7 @@
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
-      <c r="D23" s="44"/>
+      <c r="D23" s="43"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
@@ -1135,10 +1134,10 @@
       <c r="Z23" s="4"/>
     </row>
     <row r="24">
-      <c r="A24" s="45"/>
+      <c r="A24" s="44"/>
       <c r="B24" s="2"/>
       <c r="C24" s="3"/>
-      <c r="D24" s="44"/>
+      <c r="D24" s="43"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
@@ -1163,10 +1162,10 @@
       <c r="Z24" s="4"/>
     </row>
     <row r="25">
-      <c r="A25" s="45"/>
+      <c r="A25" s="44"/>
       <c r="B25" s="2"/>
       <c r="C25" s="3"/>
-      <c r="D25" s="44"/>
+      <c r="D25" s="43"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
@@ -1331,8 +1330,8 @@
       <c r="Z30" s="4"/>
     </row>
     <row r="31">
-      <c r="A31" s="45"/>
-      <c r="B31" s="45"/>
+      <c r="A31" s="44"/>
+      <c r="B31" s="44"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>

</xml_diff>